<commit_message>
updated rankings and url patterns to prefix with 'fantasyfootball'
</commit_message>
<xml_diff>
--- a/QB.xlsx
+++ b/QB.xlsx
@@ -606,7 +606,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -621,72 +621,72 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>